<commit_message>
Made Final changes to Support Single Test file with multiple data
</commit_message>
<xml_diff>
--- a/ERP_TestCaseExecution.xlsx
+++ b/ERP_TestCaseExecution.xlsx
@@ -36,13 +36,13 @@
     <t>NumberOfLines</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t>ERP_Financial_Webservice_MainClass</t>
   </si>
   <si>
     <t>ErrorReportGeneration</t>
-  </si>
-  <si>
-    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -93,10 +93,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -371,7 +375,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -379,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -401,10 +405,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -412,7 +416,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -420,7 +424,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -428,19 +432,26 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>